<commit_message>
Add the figures and tables of evaluations
</commit_message>
<xml_diff>
--- a/ISORC2017/evaluation/DynamicConnection.xlsx
+++ b/ISORC2017/evaluation/DynamicConnection.xlsx
@@ -4,23 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$3</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$4</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$1:$L$2</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$3:$L$3</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$4:$L$4</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$A$3</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$4</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$B$1:$L$2</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$3:$L$3</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$4:$L$4</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,53 +19,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
-  <si>
-    <t>CEP:  2, REP: 5</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>CEP:  2, REP: 10</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>CEP:  2, REP: 100</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>RAM</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ROM</t>
-    <phoneticPr fontId="1"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve"> </t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>CEP:  2, REP: 2</t>
+    <t>without</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>TINET</t>
+    <t>with</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>TINET+TECS</t>
+    <t>without</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>TINET</t>
+    <t>with</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>TINET+TECS</t>
+    <t>without</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>TINET+TECS</t>
+    <t>with</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>without</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>with</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>text</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>data</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bss</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CEP:  1 REP: 5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CEP:  1 REP: 1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CEP:  2 REP: 5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CEP:  5 REP: 10</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -121,11 +125,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -168,7 +169,7 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="stacked"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -179,7 +180,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>RAM</c:v>
+                  <c:v>text</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -196,47 +197,47 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$B$1:$L$2</c:f>
+              <c:f>Sheet1!$B$1:$I$2</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>TINET</c:v>
+                    <c:v>without</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>TINET+TECS</c:v>
+                    <c:v>with</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>without</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>TINET</c:v>
+                    <c:v>with</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>TINET+TECS</c:v>
+                    <c:v>without</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>with</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>TINET</c:v>
+                    <c:v>without</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>TINET+TECS</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>TINET</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>TINET+TECS</c:v>
+                    <c:v>with</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>CEP:  2, REP: 2</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>CEP:  2, REP: 5</c:v>
+                    <c:v>CEP:  1 REP: 1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>CEP:  1 REP: 5</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>CEP:  2 REP: 5</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>CEP:  2, REP: 10</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>CEP:  2, REP: 100</c:v>
+                    <c:v>CEP:  5 REP: 10</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -244,40 +245,40 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$L$3</c:f>
+              <c:f>Sheet1!$B$3:$I$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>170.32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45</c:v>
+                  <c:v>170.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>170.51300000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>170.88900000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>170.98</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>171.33</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50</c:v>
+                  <c:v>171.78</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>120</c:v>
+                  <c:v>171.97</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B756-4A4B-8702-343AB067D3D3}"/>
+              <c16:uniqueId val="{00000000-A753-46B9-8194-3EC75F0D2EC4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -290,7 +291,120 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ROM</c:v>
+                  <c:v>data</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$B$1:$I$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>without</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>with</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>without</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>with</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>without</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>with</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>without</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>with</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>CEP:  1 REP: 1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>CEP:  1 REP: 5</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>CEP:  2 REP: 5</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>CEP:  5 REP: 10</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.37</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.37</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.37</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.37</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.37</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.37</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A753-46B9-8194-3EC75F0D2EC4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>bss</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -307,47 +421,47 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$B$1:$L$2</c:f>
+              <c:f>Sheet1!$B$1:$I$2</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>TINET</c:v>
+                    <c:v>without</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>TINET+TECS</c:v>
+                    <c:v>with</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>without</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>TINET</c:v>
+                    <c:v>with</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>TINET+TECS</c:v>
+                    <c:v>without</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>with</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>TINET</c:v>
+                    <c:v>without</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>TINET+TECS</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>TINET</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>TINET+TECS</c:v>
+                    <c:v>with</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>CEP:  2, REP: 2</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>CEP:  2, REP: 5</c:v>
+                    <c:v>CEP:  1 REP: 1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>CEP:  1 REP: 5</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>CEP:  2 REP: 5</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>CEP:  2, REP: 10</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>CEP:  2, REP: 100</c:v>
+                    <c:v>CEP:  5 REP: 10</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -355,40 +469,40 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$L$4</c:f>
+              <c:f>Sheet1!$B$5:$I$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>76</c:v>
+                  <c:v>149.09599999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80</c:v>
+                  <c:v>149.09599999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>149.15599999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80</c:v>
+                  <c:v>149.166</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>90</c:v>
+                  <c:v>150.43599999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150.446</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>90</c:v>
+                  <c:v>154.32599999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>600</c:v>
+                  <c:v>154.34599999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-B756-4A4B-8702-343AB067D3D3}"/>
+              <c16:uniqueId val="{00000002-A753-46B9-8194-3EC75F0D2EC4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -400,13 +514,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
-        <c:axId val="1395362032"/>
-        <c:axId val="1383719776"/>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="113876975"/>
+        <c:axId val="113877391"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1395362032"/>
+        <c:axId val="113876975"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -449,7 +563,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1383719776"/>
+        <c:crossAx val="113877391"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -457,7 +571,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1383719776"/>
+        <c:axId val="113877391"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -477,6 +591,63 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>Size [KB]</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ja-JP"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -508,7 +679,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1395362032"/>
+        <c:crossAx val="113876975"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -630,7 +801,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -834,23 +1005,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -955,8 +1125,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1088,20 +1258,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1138,20 +1307,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:rowOff>195262</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="グラフ 2"/>
+        <xdr:cNvPr id="2" name="グラフ 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1432,133 +1601,250 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L4"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="3" t="s">
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <f>B8-39.03</f>
+        <v>170.32</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:I3" si="0">C8-39.03</f>
+        <v>170.7</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>170.51300000000001</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>170.88900000000001</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>170.98</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>171.33</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>171.78</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>171.97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>5.37</v>
+      </c>
+      <c r="C4">
+        <v>5.37</v>
+      </c>
+      <c r="D4">
+        <v>5.37</v>
+      </c>
+      <c r="E4">
+        <v>5.37</v>
+      </c>
+      <c r="F4">
+        <v>5.37</v>
+      </c>
+      <c r="G4">
+        <v>5.37</v>
+      </c>
+      <c r="H4">
+        <v>5.37</v>
+      </c>
+      <c r="I4">
+        <v>5.37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <f>B10-0.324</f>
+        <v>149.09599999999998</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:I5" si="1">C10-0.324</f>
+        <v>149.09599999999998</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>149.15599999999998</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>149.166</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>150.43599999999998</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>150.446</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>154.32599999999999</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>154.34599999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="B8">
+        <v>209.35</v>
+      </c>
+      <c r="C8">
+        <v>209.73</v>
+      </c>
+      <c r="D8">
+        <v>209.54300000000001</v>
+      </c>
+      <c r="E8">
+        <v>209.91900000000001</v>
+      </c>
+      <c r="F8">
+        <v>210.01</v>
+      </c>
+      <c r="G8">
+        <v>210.36</v>
+      </c>
+      <c r="H8">
+        <v>210.81</v>
+      </c>
+      <c r="I8">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="B9">
+        <v>5.37</v>
+      </c>
+      <c r="C9">
+        <v>5.37</v>
+      </c>
+      <c r="D9">
+        <v>5.37</v>
+      </c>
+      <c r="E9">
+        <v>5.37</v>
+      </c>
+      <c r="F9">
+        <v>5.37</v>
+      </c>
+      <c r="G9">
+        <v>5.37</v>
+      </c>
+      <c r="H9">
+        <v>5.37</v>
+      </c>
+      <c r="I9">
+        <v>5.37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="B10">
+        <v>149.41999999999999</v>
+      </c>
+      <c r="C10">
+        <v>149.41999999999999</v>
+      </c>
+      <c r="D10">
+        <v>149.47999999999999</v>
+      </c>
+      <c r="E10">
+        <v>149.49</v>
+      </c>
+      <c r="F10">
+        <v>150.76</v>
+      </c>
+      <c r="G10">
+        <v>150.77000000000001</v>
+      </c>
+      <c r="H10">
+        <v>154.65</v>
+      </c>
+      <c r="I10">
+        <v>154.66999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="J12" t="s">
         <v>0</v>
-      </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>25</v>
-      </c>
-      <c r="C3">
-        <v>45</v>
-      </c>
-      <c r="E3">
-        <v>30</v>
-      </c>
-      <c r="F3">
-        <v>50</v>
-      </c>
-      <c r="H3">
-        <v>50</v>
-      </c>
-      <c r="I3">
-        <v>69</v>
-      </c>
-      <c r="K3">
-        <v>100</v>
-      </c>
-      <c r="L3">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>76</v>
-      </c>
-      <c r="C4">
-        <v>80</v>
-      </c>
-      <c r="E4">
-        <v>80</v>
-      </c>
-      <c r="F4">
-        <v>90</v>
-      </c>
-      <c r="H4">
-        <v>90</v>
-      </c>
-      <c r="I4">
-        <v>100</v>
-      </c>
-      <c r="K4">
-        <v>500</v>
-      </c>
-      <c r="L4">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="M12" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>